<commit_message>
Cambio de formato del xlsx de edificios, para que los dias tengan tildes donde corresponda. Compliant with UI's design for days
</commit_message>
<xml_diff>
--- a/src/asignacion_aulica/data/edificios.xlsx
+++ b/src/asignacion_aulica/data/edificios.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Martes</t>
   </si>
   <si>
-    <t xml:space="preserve">Miercoles</t>
+    <t xml:space="preserve">Miércoles</t>
   </si>
   <si>
     <t xml:space="preserve">Jueves</t>
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Viernes</t>
   </si>
   <si>
-    <t xml:space="preserve">Sabado</t>
+    <t xml:space="preserve">Sábado</t>
   </si>
   <si>
     <t xml:space="preserve">Domingo</t>
@@ -79,6 +79,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -99,6 +100,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -143,12 +145,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -172,115 +178,115 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="0" t="s">
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modificacion a los datos por defecto en edificios para que no incluyan comillas. Error previo mio
</commit_message>
<xml_diff>
--- a/src/asignacion_aulica/data/edificios.xlsx
+++ b/src/asignacion_aulica/data/edificios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t xml:space="preserve">Nombre del Edificio</t>
   </si>
@@ -49,10 +49,13 @@
     <t xml:space="preserve">Anasagasti 1</t>
   </si>
   <si>
-    <t xml:space="preserve">"9:00-18:00" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"12:00-21:00" </t>
+    <t xml:space="preserve">9:00-18:00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:00-21:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:00-21:00 </t>
   </si>
   <si>
     <t xml:space="preserve">CERRADO</t>
@@ -61,10 +64,22 @@
     <t xml:space="preserve">Anasagasti 2</t>
   </si>
   <si>
-    <t xml:space="preserve">"9:00-12:00" </t>
+    <t xml:space="preserve">10:00-18:00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00-18:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00-12:00 </t>
   </si>
   <si>
     <t xml:space="preserve">Mitre 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:00-18:00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00-12:00</t>
   </si>
 </sst>
 </file>
@@ -178,7 +193,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -226,7 +241,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>9</v>
@@ -235,41 +250,41 @@
         <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>10</v>
@@ -278,16 +293,16 @@
         <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="47.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>